<commit_message>
WIP: Last working copy (with surrounding circles)
</commit_message>
<xml_diff>
--- a/hierarchy.xlsx
+++ b/hierarchy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3a3de8e06b2dcfb/Desktop/github/graph_tutorials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfhar\OneDrive\Desktop\github\graph_tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{562278D0-D27A-4D15-8823-BC535BFBD655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BEF50EA-2F56-4006-ABEC-5A2EC251263C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455A78DE-2ADB-45DA-BC59-60116E4AC80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="21426" windowHeight="11856" activeTab="2" xr2:uid="{B86EE24B-C7C4-4D9D-9299-24E98BB7EE5F}"/>
+    <workbookView xWindow="10122" yWindow="1248" windowWidth="12120" windowHeight="11988" activeTab="2" xr2:uid="{B86EE24B-C7C4-4D9D-9299-24E98BB7EE5F}"/>
   </bookViews>
   <sheets>
     <sheet name="L12A" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>A1</t>
   </si>
@@ -46,9 +46,6 @@
     <t>A2</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>A3</t>
   </si>
   <si>
@@ -110,6 +107,12 @@
   </si>
   <si>
     <t>T8</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>T10</t>
   </si>
 </sst>
 </file>
@@ -171,10 +174,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,25 +493,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611DB1BD-3106-49D1-800A-82C89C927CAC}">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.9453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -520,7 +522,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -528,18 +530,26 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -550,20 +560,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BCF31D-1A98-43D9-A27A-24F03711200A}">
-  <dimension ref="B3:C5"/>
+  <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -571,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -579,7 +589,15 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -589,10 +607,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC72E0F-A278-4BD1-8B0A-5B4E51FFB0EE}">
-  <dimension ref="B3:D18"/>
+  <dimension ref="B3:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -603,21 +621,21 @@
   <sheetData>
     <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -625,10 +643,10 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -636,7 +654,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -647,7 +665,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -658,10 +676,10 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -669,10 +687,10 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -680,21 +698,21 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -702,21 +720,21 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
         <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -724,10 +742,10 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -735,10 +753,10 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -746,10 +764,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -757,12 +775,23 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP: added more write surround and the automatic closing
</commit_message>
<xml_diff>
--- a/hierarchy.xlsx
+++ b/hierarchy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfhar\OneDrive\Desktop\github\graph_tutorials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3a3de8e06b2dcfb/Desktop/github/graph_tutorials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455A78DE-2ADB-45DA-BC59-60116E4AC80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{455A78DE-2ADB-45DA-BC59-60116E4AC80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBD5E630-EC27-4813-8A45-602329DDD931}"/>
   <bookViews>
-    <workbookView xWindow="10122" yWindow="1248" windowWidth="12120" windowHeight="11988" activeTab="2" xr2:uid="{B86EE24B-C7C4-4D9D-9299-24E98BB7EE5F}"/>
+    <workbookView xWindow="10122" yWindow="1248" windowWidth="12120" windowHeight="11988" activeTab="1" xr2:uid="{B86EE24B-C7C4-4D9D-9299-24E98BB7EE5F}"/>
   </bookViews>
   <sheets>
     <sheet name="L12A" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>A1</t>
   </si>
@@ -112,7 +112,19 @@
     <t>A10</t>
   </si>
   <si>
-    <t>T10</t>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
   </si>
 </sst>
 </file>
@@ -562,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BCF31D-1A98-43D9-A27A-24F03711200A}">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -594,10 +606,10 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -607,10 +619,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC72E0F-A278-4BD1-8B0A-5B4E51FFB0EE}">
-  <dimension ref="B3:D19"/>
+  <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -701,40 +713,40 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -742,10 +754,10 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -753,35 +765,35 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
@@ -789,9 +801,64 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
         <v>22</v>
       </c>
-      <c r="D19">
+      <c r="D24">
         <v>0</v>
       </c>
     </row>

</xml_diff>